<commit_message>
Tech report v1 done
</commit_message>
<xml_diff>
--- a/T1.xlsx
+++ b/T1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Desktop\Project Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Desktop\singhalpriyank\ProjectF13\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +165,13 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -209,10 +216,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -222,9 +230,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -274,11 +284,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Modified</a:t>
+              <a:t>Users who modified</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Privacy in some way</a:t>
+              <a:t> privacy and took at least one of the other actions</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -319,7 +329,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
-        <c:grouping val="percentStacked"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -460,7 +470,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>No</c:v>
+                  <c:v>Unsure</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -563,19 +573,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -590,7 +600,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unsure</c:v>
+                  <c:v>No</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -693,19 +703,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -721,11 +731,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1021546688"/>
-        <c:axId val="-1021546144"/>
+        <c:axId val="1332909696"/>
+        <c:axId val="1332903712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1021546688"/>
+        <c:axId val="1332909696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +763,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -768,7 +778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021546144"/>
+        <c:crossAx val="1332903712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -776,11 +786,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1021546144"/>
+        <c:axId val="1332903712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0.8"/>
+          <c:min val="65"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -798,7 +807,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> users</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -829,9 +899,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1021546688"/>
+        <c:crossAx val="1332909696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1460,15 +1531,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>361949</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1815,7 +1886,7 @@
   <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3854,10 +3925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3901,42 +3972,64 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
       <c r="F4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>0</v>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <f>B3/SUM(B3:B5)</f>
+        <v>0.95348837209302328</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" ref="C8:F8" si="0">C3/SUM(C3:C5)</f>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.97101449275362317</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.97560975609756095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>